<commit_message>
user can add the surcharge in a new line
</commit_message>
<xml_diff>
--- a/backend/static/Invoice Template.xlsx
+++ b/backend/static/Invoice Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongxiaomu/Desktop/iMIS/backend/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AA92BF-7BAF-564C-8FB5-F2379382709F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495B8D51-99B9-D846-9CE1-6D7A7A1D967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>ITE, INC.</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>BASIC</t>
-  </si>
-  <si>
-    <t>W/SUR</t>
   </si>
   <si>
     <t>INVOICE NUMBER:</t>
@@ -681,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -784,88 +781,87 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1226,7 +1222,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1263,7 +1259,7 @@
     <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="6"/>
@@ -1279,15 +1275,15 @@
       <c r="N2" s="9"/>
       <c r="O2" s="8"/>
       <c r="P2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="63"/>
+        <v>15</v>
+      </c>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="77"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
@@ -1303,15 +1299,15 @@
       <c r="N3" s="9"/>
       <c r="O3" s="8"/>
       <c r="P3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="59"/>
+        <v>16</v>
+      </c>
+      <c r="Q3" s="83"/>
+      <c r="R3" s="84"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
@@ -1354,70 +1350,70 @@
       <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
       <c r="M6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="7"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="81"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="7"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="69"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="7"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1427,67 +1423,67 @@
       <c r="M10" s="13"/>
       <c r="N10" s="14"/>
       <c r="O10" s="13"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="78"/>
+      <c r="R10" s="78"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65" t="s">
+      <c r="G11" s="59"/>
+      <c r="H11" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="59"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="63" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="64"/>
+      <c r="O11" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" s="64"/>
+    </row>
+    <row r="12" spans="1:18" s="35" customFormat="1" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="61"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="65"/>
-      <c r="H11" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="71"/>
-      <c r="O11" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="71"/>
-    </row>
-    <row r="12" spans="1:18" s="35" customFormat="1" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="74"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="64"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="31"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="68"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="65"/>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" s="16"/>
@@ -1510,34 +1506,34 @@
       <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="68"/>
+      <c r="G14" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="78"/>
-      <c r="G14" s="83" t="s">
+      <c r="H14" s="75"/>
+      <c r="I14" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="83"/>
-      <c r="I14" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14" s="81" t="s">
+      <c r="J14" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="71" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="19" t="s">
@@ -1550,30 +1546,30 @@
         <v>9</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q14" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="R14" s="72" t="s">
-        <v>32</v>
+      <c r="R14" s="57" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15" s="57"/>
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="79"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="82"/>
-      <c r="L15" s="82"/>
+        <v>26</v>
+      </c>
+      <c r="E15" s="69"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
       <c r="M15" s="15" t="s">
         <v>4</v>
       </c>
@@ -1584,12 +1580,10 @@
         <v>10</v>
       </c>
       <c r="P15" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="R15" s="73"/>
+        <v>18</v>
+      </c>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="58"/>
     </row>
     <row r="16" spans="1:18" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -1609,15 +1603,15 @@
       <c r="M16" s="13"/>
       <c r="N16" s="14"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="84" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" s="85"/>
+      <c r="P16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="56"/>
       <c r="R16" s="27"/>
     </row>
     <row r="17" spans="1:14" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A17" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
@@ -1629,36 +1623,36 @@
       <c r="I17" s="52"/>
       <c r="J17" s="53"/>
       <c r="K17" s="50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A18" s="46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="47"/>
       <c r="C18" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="47"/>
       <c r="E18" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F18" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="34" t="s">
+      <c r="H18" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="I18" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="J18" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="J18" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="N18" s="3"/>
     </row>
@@ -1690,7 +1684,29 @@
     </row>
     <row r="21" spans="1:14" ht="14" thickTop="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="38">
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="N7:R7"/>
+    <mergeCell ref="N8:R8"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="R14:R15"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="F12:G12"/>
@@ -1706,28 +1722,7 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="G14:H15"/>
     <mergeCell ref="E14:F15"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="N7:R7"/>
-    <mergeCell ref="N8:R8"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="I14:I15"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="J14:J15"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>

</xml_diff>